<commit_message>
Style footer and button
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,59 +1,133 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B412B847-DEEE-4A05-B0B4-CBDD93D9989D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="4605" yWindow="1530" windowWidth="24060" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Site Data" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Site Data" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <family val="2"/>
+            <sz val="12"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Require column</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <family val="2"/>
+            <sz val="12"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Require column</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <family val="2"/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Optional column</t>
+        </r>
+        <r>
+          <rPr>
+            <color theme="1"/>
+            <sz val="10"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+If there is no column, it will not be filled</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>rewrite header</t>
-  </si>
-  <si>
-    <t>13.10.2023, 15:31:23</t>
-  </si>
-  <si>
-    <t>url1</t>
-  </si>
-  <si>
-    <t>url2</t>
-  </si>
-  <si>
-    <t>url3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+  <si>
+    <t>Some info</t>
+  </si>
+  <si>
+    <t>Site URL</t>
+  </si>
+  <si>
+    <t>Thematicity Index</t>
+  </si>
+  <si>
+    <t>Total Page</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>washingtonpost.com</t>
+  </si>
+  <si>
+    <t>will be filled</t>
+  </si>
+  <si>
+    <t>www.businessinsider.com/</t>
+  </si>
+  <si>
+    <t>https://www.who.int/</t>
+  </si>
+  <si>
+    <t>macobserver.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6E0B4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,11 +142,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -408,56 +495,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="10" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>5</v>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish Excel read function
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,62 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F09E848-1EEB-427F-BD94-2AFB88872A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-25605" yWindow="3780" windowWidth="24060" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Site Data" state="visible" r:id="rId4"/>
+    <sheet name="Site Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Author</author>
+    <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
-            <family val="2"/>
             <sz val="12"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Require column</t>
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
-            <family val="2"/>
             <sz val="12"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Require column</t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
             <b/>
-            <family val="2"/>
             <sz val="11"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Optional column</t>
         </r>
         <r>
           <rPr>
+            <sz val="10"/>
             <color theme="1"/>
-            <sz val="10"/>
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
@@ -69,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t>Some info</t>
   </si>
@@ -104,17 +108,57 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₴&quot;_-;\-* #,##0.00\ &quot;₴&quot;_-;_-* &quot;-&quot;??\ &quot;₴&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Adobe Fan Heiti Std B"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="3">
@@ -126,7 +170,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="C6E0B4"/>
+        <fgColor rgb="FFC6E0B4"/>
       </patternFill>
     </fill>
   </fills>
@@ -139,10 +183,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,9 +203,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Грошовий" xfId="2" builtinId="4"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Фінансовий" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -495,9 +553,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
@@ -507,7 +570,7 @@
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -527,7 +590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -543,11 +606,11 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>6</v>
+      <c r="F2" s="6">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -563,11 +626,11 @@
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>6</v>
+      <c r="F3" s="8">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -583,11 +646,11 @@
       <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>6</v>
+      <c r="F4" s="9">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -603,13 +666,15 @@
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="F5" s="5">
+        <f>2 + 2</f>
+        <v>4</v>
+      </c>
+      <c r="I5" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>